<commit_message>
added few more componenets
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iterationdata" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="runmanager" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -103,6 +103,60 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>test description 1</t>
+  </si>
+  <si>
+    <t>test description 2</t>
+  </si>
+  <si>
+    <t>postRequestUsingPojo</t>
+  </si>
+  <si>
+    <t>test description 3</t>
+  </si>
+  <si>
+    <t>skjdbv</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>tester,trainer,farmer</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>idly</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>pizza</t>
+  </si>
+  <si>
+    <t>postRequestUsingPojoAndBuilders</t>
+  </si>
+  <si>
+    <t>kskdjc</t>
+  </si>
+  <si>
+    <t>tester,trainer</t>
+  </si>
+  <si>
+    <t>test description 4 --&gt; I will be logged in the extent report</t>
   </si>
 </sst>
 </file>
@@ -435,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -446,10 +500,11 @@
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -469,10 +524,22 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -492,10 +559,22 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -515,10 +594,22 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -538,10 +629,22 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -561,10 +664,22 @@
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -584,10 +699,22 @@
         <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -609,8 +736,20 @@
       <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -631,6 +770,88 @@
       </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -641,12 +862,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>